<commit_message>
first draft to include sepia as a snakemake job
</commit_message>
<xml_diff>
--- a/SEPIA/COUNTRIES.xlsx
+++ b/SEPIA/COUNTRIES.xlsx
@@ -108,7 +108,7 @@
     <t xml:space="preserve">BE</t>
   </si>
   <si>
-    <t xml:space="preserve">inputs_BE</t>
+    <t xml:space="preserve">inputsBE</t>
   </si>
   <si>
     <t xml:space="preserve">Belgium</t>
@@ -177,7 +177,7 @@
     <t xml:space="preserve">DE</t>
   </si>
   <si>
-    <t xml:space="preserve">inputs_DE</t>
+    <t xml:space="preserve">inputsDE</t>
   </si>
   <si>
     <t xml:space="preserve">Germany</t>
@@ -264,7 +264,7 @@
     <t xml:space="preserve">FR</t>
   </si>
   <si>
-    <t xml:space="preserve">inputs_FR</t>
+    <t xml:space="preserve">inputsFR</t>
   </si>
   <si>
     <t xml:space="preserve">France</t>
@@ -381,7 +381,7 @@
     <t xml:space="preserve">NL</t>
   </si>
   <si>
-    <t xml:space="preserve">inputs_NL</t>
+    <t xml:space="preserve">inputsNL</t>
   </si>
   <si>
     <t xml:space="preserve">Netherlands</t>
@@ -483,7 +483,7 @@
     <t xml:space="preserve">GB</t>
   </si>
   <si>
-    <t xml:space="preserve">inputs_GB</t>
+    <t xml:space="preserve">inputsGB</t>
   </si>
   <si>
     <t xml:space="preserve">United Kingdom</t>
@@ -602,7 +602,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -612,10 +612,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -789,7 +785,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.62"/>
@@ -828,7 +824,7 @@
       <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="b">
+      <c r="B4" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -840,7 +836,7 @@
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="b">
+      <c r="B5" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -852,7 +848,7 @@
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="b">
+      <c r="B6" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -931,10 +927,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.91"/>
@@ -969,13 +965,13 @@
       <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="5"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -998,7 +994,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H2" s="6" t="str">
+      <c r="H2" s="5" t="str">
         <f aca="false">$I2</f>
         <v>Dashboard_AT_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1006,7 +1002,7 @@
         <f aca="false">"Dashboard_"&amp;$A2&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_AT_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J2" s="6" t="str">
+      <c r="J2" s="5" t="str">
         <f aca="false">H2</f>
         <v>Dashboard_AT_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1035,14 +1031,14 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="I3" s="0" t="str">
         <f aca="false">"Dashboard_"&amp;$A3&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_BE_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J3" s="8" t="str">
+      <c r="J3" s="7" t="str">
         <f aca="false">H3</f>
         <v>Dashboard_BE_v5.13</v>
       </c>
@@ -1068,7 +1064,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H4" s="8" t="str">
+      <c r="H4" s="7" t="str">
         <f aca="false">$I4</f>
         <v>Dashboard_BG_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1076,7 +1072,7 @@
         <f aca="false">"Dashboard_"&amp;$A4&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_BG_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J4" s="8" t="str">
+      <c r="J4" s="7" t="str">
         <f aca="false">H4</f>
         <v>Dashboard_BG_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1102,7 +1098,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H5" s="6" t="str">
+      <c r="H5" s="5" t="str">
         <f aca="false">I5</f>
         <v>Dashboard_CH_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1110,7 +1106,7 @@
         <f aca="false">"Dashboard_"&amp;$A5&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_CH_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="8" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1135,7 +1131,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H6" s="8" t="str">
+      <c r="H6" s="7" t="str">
         <f aca="false">$I6</f>
         <v>Dashboard_CY_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1143,7 +1139,7 @@
         <f aca="false">"Dashboard_"&amp;$A6&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_CY_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J6" s="8" t="str">
+      <c r="J6" s="7" t="str">
         <f aca="false">H6</f>
         <v>Dashboard_CY_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1169,7 +1165,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H7" s="8" t="str">
+      <c r="H7" s="7" t="str">
         <f aca="false">$I7</f>
         <v>Dashboard_CZ_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1177,7 +1173,7 @@
         <f aca="false">"Dashboard_"&amp;$A7&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_CZ_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J7" s="8" t="str">
+      <c r="J7" s="7" t="str">
         <f aca="false">H7</f>
         <v>Dashboard_CZ_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1198,22 +1194,22 @@
       <c r="E8" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G8" s="3" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H8" s="9" t="s">
+      <c r="F8" s="2" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>53</v>
       </c>
       <c r="I8" s="0" t="str">
         <f aca="false">"Dashboard_"&amp;$A8&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_DE_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J8" s="8" t="str">
+      <c r="J8" s="7" t="str">
         <f aca="false">H8</f>
         <v>Dashboard_DE_v5.9</v>
       </c>
@@ -1235,11 +1231,11 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G9" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="6" t="str">
+      <c r="G9" s="2" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="5" t="str">
         <f aca="false">$I9</f>
         <v>Dashboard_DK_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1247,7 +1243,7 @@
         <f aca="false">"Dashboard_"&amp;$A9&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_DK_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="8" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1272,7 +1268,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H10" s="8" t="str">
+      <c r="H10" s="7" t="str">
         <f aca="false">$I10</f>
         <v>Dashboard_EE_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1280,7 +1276,7 @@
         <f aca="false">"Dashboard_"&amp;$A10&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_EE_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J10" s="8" t="str">
+      <c r="J10" s="7" t="str">
         <f aca="false">H10</f>
         <v>Dashboard_EE_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1306,7 +1302,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H11" s="8" t="str">
+      <c r="H11" s="7" t="str">
         <f aca="false">$I11</f>
         <v>Dashboard_EL_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1314,7 +1310,7 @@
         <f aca="false">"Dashboard_"&amp;$A11&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_EL_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1322,7 +1318,7 @@
       <c r="A12" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="0" t="s">
         <v>69</v>
       </c>
@@ -1340,14 +1336,14 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="6" t="s">
         <v>72</v>
       </c>
       <c r="I12" s="0" t="str">
         <f aca="false">"Dashboard_"&amp;$A12&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_ES_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J12" s="8" t="str">
+      <c r="J12" s="7" t="str">
         <f aca="false">H12</f>
         <v>Dashboard_ES_v5.16</v>
       </c>
@@ -1373,7 +1369,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H13" s="8" t="str">
+      <c r="H13" s="7" t="str">
         <f aca="false">$I13</f>
         <v>Dashboard_FI_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1381,7 +1377,7 @@
         <f aca="false">"Dashboard_"&amp;$A13&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_FI_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J13" s="8" t="str">
+      <c r="J13" s="7" t="str">
         <f aca="false">H13</f>
         <v>Dashboard_FI_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1410,14 +1406,14 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="8" t="s">
         <v>82</v>
       </c>
       <c r="I14" s="0" t="str">
         <f aca="false">"Dashboard_"&amp;$A14&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_FR_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J14" s="8" t="str">
+      <c r="J14" s="7" t="str">
         <f aca="false">H14</f>
         <v>Dashboard_FR_v5.12</v>
       </c>
@@ -1443,7 +1439,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H15" s="8" t="str">
+      <c r="H15" s="7" t="str">
         <f aca="false">$I15</f>
         <v>Dashboard_HR_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1451,7 +1447,7 @@
         <f aca="false">"Dashboard_"&amp;$A15&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_HR_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J15" s="8" t="str">
+      <c r="J15" s="7" t="str">
         <f aca="false">H15</f>
         <v>Dashboard_HR_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1477,7 +1473,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H16" s="6" t="str">
+      <c r="H16" s="5" t="str">
         <f aca="false">$I16</f>
         <v>Dashboard_HU_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1485,7 +1481,7 @@
         <f aca="false">"Dashboard_"&amp;$A16&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_HU_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J16" s="8" t="str">
+      <c r="J16" s="7" t="str">
         <f aca="false">H16</f>
         <v>Dashboard_HU_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1511,7 +1507,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H17" s="8" t="str">
+      <c r="H17" s="7" t="str">
         <f aca="false">$I17</f>
         <v>Dashboard_IE_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1519,7 +1515,7 @@
         <f aca="false">"Dashboard_"&amp;$A17&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_IE_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J17" s="8" t="str">
+      <c r="J17" s="7" t="str">
         <f aca="false">H17</f>
         <v>Dashboard_IE_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1545,14 +1541,14 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="8" t="s">
         <v>99</v>
       </c>
       <c r="I18" s="0" t="str">
         <f aca="false">"Dashboard_"&amp;$A18&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_IT_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J18" s="8" t="str">
+      <c r="J18" s="7" t="str">
         <f aca="false">H18</f>
         <v>Dashboard_IT_v5.10</v>
       </c>
@@ -1578,7 +1574,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H19" s="8" t="str">
+      <c r="H19" s="7" t="str">
         <f aca="false">$I19</f>
         <v>Dashboard_LT_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1586,7 +1582,7 @@
         <f aca="false">"Dashboard_"&amp;$A19&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_LT_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J19" s="8" t="str">
+      <c r="J19" s="7" t="str">
         <f aca="false">H19</f>
         <v>Dashboard_LT_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1612,7 +1608,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H20" s="8" t="str">
+      <c r="H20" s="7" t="str">
         <f aca="false">$I20</f>
         <v>Dashboard_LU_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1620,7 +1616,7 @@
         <f aca="false">"Dashboard_"&amp;$A20&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_LU_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J20" s="8" t="str">
+      <c r="J20" s="7" t="str">
         <f aca="false">H20</f>
         <v>Dashboard_LU_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1646,7 +1642,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H21" s="8" t="str">
+      <c r="H21" s="7" t="str">
         <f aca="false">$I21</f>
         <v>Dashboard_LV_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1654,7 +1650,7 @@
         <f aca="false">"Dashboard_"&amp;$A21&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_LV_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J21" s="8" t="str">
+      <c r="J21" s="7" t="str">
         <f aca="false">H21</f>
         <v>Dashboard_LV_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1680,7 +1676,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H22" s="8" t="str">
+      <c r="H22" s="7" t="str">
         <f aca="false">$I22</f>
         <v>Dashboard_MT_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1688,7 +1684,7 @@
         <f aca="false">"Dashboard_"&amp;$A22&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_MT_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J22" s="8" t="str">
+      <c r="J22" s="7" t="str">
         <f aca="false">H22</f>
         <v>Dashboard_MT_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1717,7 +1713,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H23" s="8" t="str">
+      <c r="H23" s="7" t="str">
         <f aca="false">$I23</f>
         <v>Dashboard_NL_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1725,7 +1721,7 @@
         <f aca="false">"Dashboard_"&amp;$A23&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_NL_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J23" s="8" t="str">
+      <c r="J23" s="7" t="str">
         <f aca="false">H23</f>
         <v>Dashboard_NL_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1751,7 +1747,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H24" s="8" t="str">
+      <c r="H24" s="7" t="str">
         <f aca="false">$I24</f>
         <v>Dashboard_NO_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1759,7 +1755,7 @@
         <f aca="false">"Dashboard_"&amp;$A24&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_NO_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J24" s="6" t="str">
+      <c r="J24" s="5" t="str">
         <f aca="false">H24</f>
         <v>Dashboard_NO_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1785,7 +1781,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H25" s="8" t="str">
+      <c r="H25" s="7" t="str">
         <f aca="false">$I25</f>
         <v>Dashboard_PL_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1793,7 +1789,7 @@
         <f aca="false">"Dashboard_"&amp;$A25&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_PL_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J25" s="8" t="str">
+      <c r="J25" s="7" t="str">
         <f aca="false">H25</f>
         <v>Dashboard_PL_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1819,7 +1815,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H26" s="8" t="str">
+      <c r="H26" s="7" t="str">
         <f aca="false">$I26</f>
         <v>Dashboard_PT_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1827,7 +1823,7 @@
         <f aca="false">"Dashboard_"&amp;$A26&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_PT_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J26" s="9" t="s">
+      <c r="J26" s="8" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1852,7 +1848,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H27" s="8" t="str">
+      <c r="H27" s="7" t="str">
         <f aca="false">$I27</f>
         <v>Dashboard_RO_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1860,7 +1856,7 @@
         <f aca="false">"Dashboard_"&amp;$A27&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_RO_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J27" s="8" t="str">
+      <c r="J27" s="7" t="str">
         <f aca="false">H27</f>
         <v>Dashboard_RO_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1886,7 +1882,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H28" s="8" t="str">
+      <c r="H28" s="7" t="str">
         <f aca="false">$I28</f>
         <v>Dashboard_SE_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1894,7 +1890,7 @@
         <f aca="false">"Dashboard_"&amp;$A28&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_SE_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J28" s="9" t="s">
+      <c r="J28" s="8" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1919,7 +1915,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H29" s="8" t="str">
+      <c r="H29" s="7" t="str">
         <f aca="false">$I29</f>
         <v>Dashboard_SI_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1927,7 +1923,7 @@
         <f aca="false">"Dashboard_"&amp;$A29&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_SI_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J29" s="8" t="str">
+      <c r="J29" s="7" t="str">
         <f aca="false">H29</f>
         <v>Dashboard_SI_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1953,7 +1949,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H30" s="8" t="str">
+      <c r="H30" s="7" t="str">
         <f aca="false">$I30</f>
         <v>Dashboard_SK_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1961,7 +1957,7 @@
         <f aca="false">"Dashboard_"&amp;$A30&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_SK_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J30" s="8" t="str">
+      <c r="J30" s="7" t="str">
         <f aca="false">H30</f>
         <v>Dashboard_SK_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1990,7 +1986,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H31" s="8" t="str">
+      <c r="H31" s="7" t="str">
         <f aca="false">$I31</f>
         <v>Dashboard_GB_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1998,7 +1994,7 @@
         <f aca="false">"Dashboard_"&amp;$A31&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_GB_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J31" s="6" t="str">
+      <c r="J31" s="5" t="str">
         <f aca="false">H31</f>
         <v>Dashboard_GB_v5.19_PNC_Tra_Int</v>
       </c>

</xml_diff>

<commit_message>
removing errors for bau scenario
</commit_message>
<xml_diff>
--- a/SEPIA/COUNTRIES.xlsx
+++ b/SEPIA/COUNTRIES.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="158">
   <si>
     <t xml:space="preserve">Column</t>
   </si>
@@ -493,6 +493,15 @@
   </si>
   <si>
     <t xml:space="preserve">GBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inputsEU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
   </si>
 </sst>
 </file>
@@ -785,7 +794,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.62"/>
@@ -860,7 +869,7 @@
       <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="b">
+      <c r="B7" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -872,7 +881,7 @@
       <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="b">
+      <c r="B8" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -884,7 +893,7 @@
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="0" t="b">
+      <c r="B9" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -896,7 +905,7 @@
       <c r="A10" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="0" t="b">
+      <c r="B10" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -927,10 +936,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="bottomRight" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.91"/>
@@ -1999,6 +2008,17 @@
         <v>Dashboard_GB_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:J1"/>

</xml_diff>

<commit_message>
using CLEVER LULUCF assumptions for BAU scenario + small changes
</commit_message>
<xml_diff>
--- a/SEPIA/COUNTRIES.xlsx
+++ b/SEPIA/COUNTRIES.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="181">
   <si>
     <t xml:space="preserve">Column</t>
   </si>
@@ -96,6 +96,9 @@
     <t xml:space="preserve">AT</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsAT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Austria</t>
   </si>
   <si>
@@ -126,6 +129,9 @@
     <t xml:space="preserve">BG</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsBG</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bulgaria</t>
   </si>
   <si>
@@ -138,6 +144,9 @@
     <t xml:space="preserve">CH</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsCH</t>
+  </si>
+  <si>
     <t xml:space="preserve">Switzerland</t>
   </si>
   <si>
@@ -165,6 +174,9 @@
     <t xml:space="preserve">CZ</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsCZ</t>
+  </si>
+  <si>
     <t xml:space="preserve">Czech Republic</t>
   </si>
   <si>
@@ -195,6 +207,9 @@
     <t xml:space="preserve">DK</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsDK</t>
+  </si>
+  <si>
     <t xml:space="preserve">Denmark</t>
   </si>
   <si>
@@ -210,6 +225,9 @@
     <t xml:space="preserve">EE</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsEE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Estonia</t>
   </si>
   <si>
@@ -222,6 +240,9 @@
     <t xml:space="preserve">EL</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsGR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Greece</t>
   </si>
   <si>
@@ -237,6 +258,9 @@
     <t xml:space="preserve">ES</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsES</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spain</t>
   </si>
   <si>
@@ -252,6 +276,9 @@
     <t xml:space="preserve">FI</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsFI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Finland</t>
   </si>
   <si>
@@ -282,6 +309,9 @@
     <t xml:space="preserve">HR</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsHR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Croatia</t>
   </si>
   <si>
@@ -294,6 +324,9 @@
     <t xml:space="preserve">HU</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsHU</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hungary</t>
   </si>
   <si>
@@ -306,6 +339,9 @@
     <t xml:space="preserve">IE</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsIE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ireland</t>
   </si>
   <si>
@@ -318,6 +354,9 @@
     <t xml:space="preserve">IT</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsIT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Italy</t>
   </si>
   <si>
@@ -333,6 +372,9 @@
     <t xml:space="preserve">LT</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsLT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lithuania</t>
   </si>
   <si>
@@ -345,6 +387,9 @@
     <t xml:space="preserve">LU</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsLU</t>
+  </si>
+  <si>
     <t xml:space="preserve">Luxembourg</t>
   </si>
   <si>
@@ -357,6 +402,9 @@
     <t xml:space="preserve">LV</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsLV</t>
+  </si>
+  <si>
     <t xml:space="preserve">Latvia</t>
   </si>
   <si>
@@ -396,6 +444,9 @@
     <t xml:space="preserve">NO</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsNO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Norway</t>
   </si>
   <si>
@@ -405,6 +456,9 @@
     <t xml:space="preserve">PL</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsPL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Poland</t>
   </si>
   <si>
@@ -417,6 +471,9 @@
     <t xml:space="preserve">PT</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsPT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Portugal</t>
   </si>
   <si>
@@ -432,6 +489,9 @@
     <t xml:space="preserve">RO</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsRO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Romania</t>
   </si>
   <si>
@@ -444,6 +504,9 @@
     <t xml:space="preserve">SE</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsSE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sweden</t>
   </si>
   <si>
@@ -459,6 +522,9 @@
     <t xml:space="preserve">SI</t>
   </si>
   <si>
+    <t xml:space="preserve">inputsSI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Slovenia</t>
   </si>
   <si>
@@ -469,6 +535,9 @@
   </si>
   <si>
     <t xml:space="preserve">SK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inputsSK</t>
   </si>
   <si>
     <t xml:space="preserve">Slovakia</t>
@@ -611,7 +680,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -621,6 +690,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -794,7 +867,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.62"/>
@@ -833,7 +906,7 @@
       <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="b">
+      <c r="B4" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -845,7 +918,7 @@
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="b">
+      <c r="B5" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -857,7 +930,7 @@
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="b">
+      <c r="B6" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -869,7 +942,7 @@
       <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="b">
+      <c r="B7" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -881,7 +954,7 @@
       <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="b">
+      <c r="B8" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -893,7 +966,7 @@
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="b">
+      <c r="B9" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -905,7 +978,7 @@
       <c r="A10" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="b">
+      <c r="B10" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -936,10 +1009,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C32" activeCellId="0" sqref="C32"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.91"/>
@@ -974,26 +1047,29 @@
       <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="4"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="C2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2" t="b">
         <f aca="false">TRUE()</f>
@@ -1003,7 +1079,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H2" s="5" t="str">
+      <c r="H2" s="6" t="str">
         <f aca="false">$I2</f>
         <v>Dashboard_AT_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1011,26 +1087,26 @@
         <f aca="false">"Dashboard_"&amp;$A2&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_AT_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J2" s="5" t="str">
+      <c r="J2" s="6" t="str">
         <f aca="false">H2</f>
         <v>Dashboard_AT_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F3" s="2" t="b">
         <f aca="false">TRUE()</f>
@@ -1040,30 +1116,33 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>30</v>
+      <c r="H3" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="I3" s="0" t="str">
         <f aca="false">"Dashboard_"&amp;$A3&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_BE_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J3" s="7" t="str">
+      <c r="J3" s="8" t="str">
         <f aca="false">H3</f>
         <v>Dashboard_BE_v5.13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>33</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F4" s="2" t="b">
         <f aca="false">TRUE()</f>
@@ -1073,7 +1152,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H4" s="7" t="str">
+      <c r="H4" s="8" t="str">
         <f aca="false">$I4</f>
         <v>Dashboard_BG_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1081,23 +1160,26 @@
         <f aca="false">"Dashboard_"&amp;$A4&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_BG_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J4" s="7" t="str">
+      <c r="J4" s="8" t="str">
         <f aca="false">H4</f>
         <v>Dashboard_BG_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>38</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F5" s="2" t="b">
         <f aca="false">FALSE()</f>
@@ -1107,7 +1189,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H5" s="5" t="str">
+      <c r="H5" s="6" t="str">
         <f aca="false">I5</f>
         <v>Dashboard_CH_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1115,22 +1197,22 @@
         <f aca="false">"Dashboard_"&amp;$A5&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_CH_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>39</v>
+      <c r="J5" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F6" s="2" t="b">
         <f aca="false">TRUE()</f>
@@ -1140,7 +1222,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H6" s="7" t="str">
+      <c r="H6" s="8" t="str">
         <f aca="false">$I6</f>
         <v>Dashboard_CY_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1148,23 +1230,26 @@
         <f aca="false">"Dashboard_"&amp;$A6&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_CY_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J6" s="7" t="str">
+      <c r="J6" s="8" t="str">
         <f aca="false">H6</f>
         <v>Dashboard_CY_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F7" s="2" t="b">
         <f aca="false">TRUE()</f>
@@ -1174,7 +1259,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H7" s="7" t="str">
+      <c r="H7" s="8" t="str">
         <f aca="false">$I7</f>
         <v>Dashboard_CZ_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1182,69 +1267,72 @@
         <f aca="false">"Dashboard_"&amp;$A7&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_CZ_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J7" s="7" t="str">
+      <c r="J7" s="8" t="str">
         <f aca="false">H7</f>
         <v>Dashboard_CZ_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="2" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G8" s="2" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="F8" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="I8" s="0" t="str">
         <f aca="false">"Dashboard_"&amp;$A8&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_DE_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J8" s="7" t="str">
+      <c r="J8" s="8" t="str">
         <f aca="false">H8</f>
         <v>Dashboard_DE_v5.9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F9" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G9" s="2" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="5" t="str">
+      <c r="G9" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="6" t="str">
         <f aca="false">$I9</f>
         <v>Dashboard_DK_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1252,22 +1340,25 @@
         <f aca="false">"Dashboard_"&amp;$A9&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_DK_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>58</v>
+      <c r="J9" s="9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F10" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1277,7 +1368,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H10" s="7" t="str">
+      <c r="H10" s="8" t="str">
         <f aca="false">$I10</f>
         <v>Dashboard_EE_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1285,23 +1376,26 @@
         <f aca="false">"Dashboard_"&amp;$A10&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_EE_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J10" s="7" t="str">
+      <c r="J10" s="8" t="str">
         <f aca="false">H10</f>
         <v>Dashboard_EE_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>70</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F11" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1311,7 +1405,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H11" s="7" t="str">
+      <c r="H11" s="8" t="str">
         <f aca="false">$I11</f>
         <v>Dashboard_EL_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1319,23 +1413,25 @@
         <f aca="false">"Dashboard_"&amp;$A11&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_EL_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J11" s="8" t="s">
-        <v>67</v>
+      <c r="J11" s="9" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="6"/>
+        <v>75</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>76</v>
+      </c>
       <c r="C12" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="F12" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1345,30 +1441,33 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>72</v>
+      <c r="H12" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="I12" s="0" t="str">
         <f aca="false">"Dashboard_"&amp;$A12&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_ES_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J12" s="7" t="str">
+      <c r="J12" s="8" t="str">
         <f aca="false">H12</f>
         <v>Dashboard_ES_v5.16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>82</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="F13" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1378,7 +1477,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H13" s="7" t="str">
+      <c r="H13" s="8" t="str">
         <f aca="false">$I13</f>
         <v>Dashboard_FI_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1386,26 +1485,26 @@
         <f aca="false">"Dashboard_"&amp;$A13&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_FI_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J13" s="7" t="str">
+      <c r="J13" s="8" t="str">
         <f aca="false">H13</f>
         <v>Dashboard_FI_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="F14" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1415,30 +1514,33 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>82</v>
+      <c r="H14" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="I14" s="0" t="str">
         <f aca="false">"Dashboard_"&amp;$A14&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_FR_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J14" s="7" t="str">
+      <c r="J14" s="8" t="str">
         <f aca="false">H14</f>
         <v>Dashboard_FR_v5.12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>83</v>
+        <v>92</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>93</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F15" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1448,7 +1550,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H15" s="7" t="str">
+      <c r="H15" s="8" t="str">
         <f aca="false">$I15</f>
         <v>Dashboard_HR_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1456,23 +1558,26 @@
         <f aca="false">"Dashboard_"&amp;$A15&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_HR_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J15" s="7" t="str">
+      <c r="J15" s="8" t="str">
         <f aca="false">H15</f>
         <v>Dashboard_HR_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>87</v>
+        <v>97</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>98</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="F16" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1482,7 +1587,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H16" s="5" t="str">
+      <c r="H16" s="6" t="str">
         <f aca="false">$I16</f>
         <v>Dashboard_HU_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1490,23 +1595,26 @@
         <f aca="false">"Dashboard_"&amp;$A16&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_HU_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J16" s="7" t="str">
+      <c r="J16" s="8" t="str">
         <f aca="false">H16</f>
         <v>Dashboard_HU_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>91</v>
+        <v>102</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>103</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="F17" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1516,7 +1624,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H17" s="7" t="str">
+      <c r="H17" s="8" t="str">
         <f aca="false">$I17</f>
         <v>Dashboard_IE_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1524,23 +1632,26 @@
         <f aca="false">"Dashboard_"&amp;$A17&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_IE_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J17" s="7" t="str">
+      <c r="J17" s="8" t="str">
         <f aca="false">H17</f>
         <v>Dashboard_IE_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>95</v>
+        <v>107</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>108</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="F18" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1550,30 +1661,33 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H18" s="8" t="s">
-        <v>99</v>
+      <c r="H18" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="I18" s="0" t="str">
         <f aca="false">"Dashboard_"&amp;$A18&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_IT_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J18" s="7" t="str">
+      <c r="J18" s="8" t="str">
         <f aca="false">H18</f>
         <v>Dashboard_IT_v5.10</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>100</v>
+        <v>113</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>114</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="F19" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1583,7 +1697,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H19" s="7" t="str">
+      <c r="H19" s="8" t="str">
         <f aca="false">$I19</f>
         <v>Dashboard_LT_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1591,23 +1705,26 @@
         <f aca="false">"Dashboard_"&amp;$A19&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_LT_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J19" s="7" t="str">
+      <c r="J19" s="8" t="str">
         <f aca="false">H19</f>
         <v>Dashboard_LT_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>104</v>
+        <v>118</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>119</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="F20" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1617,7 +1734,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H20" s="7" t="str">
+      <c r="H20" s="8" t="str">
         <f aca="false">$I20</f>
         <v>Dashboard_LU_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1625,23 +1742,26 @@
         <f aca="false">"Dashboard_"&amp;$A20&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_LU_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J20" s="7" t="str">
+      <c r="J20" s="8" t="str">
         <f aca="false">H20</f>
         <v>Dashboard_LU_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>108</v>
+        <v>123</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>124</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="F21" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1651,7 +1771,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H21" s="7" t="str">
+      <c r="H21" s="8" t="str">
         <f aca="false">$I21</f>
         <v>Dashboard_LV_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1659,23 +1779,23 @@
         <f aca="false">"Dashboard_"&amp;$A21&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_LV_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J21" s="7" t="str">
+      <c r="J21" s="8" t="str">
         <f aca="false">H21</f>
         <v>Dashboard_LV_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="F22" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1685,7 +1805,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H22" s="7" t="str">
+      <c r="H22" s="8" t="str">
         <f aca="false">$I22</f>
         <v>Dashboard_MT_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1693,26 +1813,26 @@
         <f aca="false">"Dashboard_"&amp;$A22&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_MT_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J22" s="7" t="str">
+      <c r="J22" s="8" t="str">
         <f aca="false">H22</f>
         <v>Dashboard_MT_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="F23" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1722,7 +1842,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H23" s="7" t="str">
+      <c r="H23" s="8" t="str">
         <f aca="false">$I23</f>
         <v>Dashboard_NL_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1730,23 +1850,26 @@
         <f aca="false">"Dashboard_"&amp;$A23&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_NL_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J23" s="7" t="str">
+      <c r="J23" s="8" t="str">
         <f aca="false">H23</f>
         <v>Dashboard_NL_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>121</v>
+        <v>137</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>138</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="F24" s="0" t="b">
         <f aca="false">FALSE()</f>
@@ -1756,7 +1879,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H24" s="7" t="str">
+      <c r="H24" s="8" t="str">
         <f aca="false">$I24</f>
         <v>Dashboard_NO_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1764,23 +1887,26 @@
         <f aca="false">"Dashboard_"&amp;$A24&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_NO_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J24" s="5" t="str">
+      <c r="J24" s="6" t="str">
         <f aca="false">H24</f>
         <v>Dashboard_NO_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>124</v>
+        <v>141</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>142</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="F25" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1790,7 +1916,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H25" s="7" t="str">
+      <c r="H25" s="8" t="str">
         <f aca="false">$I25</f>
         <v>Dashboard_PL_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1798,23 +1924,26 @@
         <f aca="false">"Dashboard_"&amp;$A25&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_PL_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J25" s="7" t="str">
+      <c r="J25" s="8" t="str">
         <f aca="false">H25</f>
         <v>Dashboard_PL_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>128</v>
+        <v>146</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>147</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="F26" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1824,7 +1953,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H26" s="7" t="str">
+      <c r="H26" s="8" t="str">
         <f aca="false">$I26</f>
         <v>Dashboard_PT_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1832,22 +1961,25 @@
         <f aca="false">"Dashboard_"&amp;$A26&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_PT_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J26" s="8" t="s">
-        <v>132</v>
+      <c r="J26" s="9" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>133</v>
+        <v>152</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>153</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="F27" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1857,7 +1989,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H27" s="7" t="str">
+      <c r="H27" s="8" t="str">
         <f aca="false">$I27</f>
         <v>Dashboard_RO_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1865,23 +1997,26 @@
         <f aca="false">"Dashboard_"&amp;$A27&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_RO_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J27" s="7" t="str">
+      <c r="J27" s="8" t="str">
         <f aca="false">H27</f>
         <v>Dashboard_RO_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>137</v>
+        <v>157</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="F28" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1891,7 +2026,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H28" s="7" t="str">
+      <c r="H28" s="8" t="str">
         <f aca="false">$I28</f>
         <v>Dashboard_SE_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1899,22 +2034,25 @@
         <f aca="false">"Dashboard_"&amp;$A28&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_SE_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J28" s="8" t="s">
-        <v>141</v>
+      <c r="J28" s="9" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>142</v>
+        <v>163</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>164</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="F29" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1924,7 +2062,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H29" s="7" t="str">
+      <c r="H29" s="8" t="str">
         <f aca="false">$I29</f>
         <v>Dashboard_SI_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1932,23 +2070,26 @@
         <f aca="false">"Dashboard_"&amp;$A29&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_SI_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J29" s="7" t="str">
+      <c r="J29" s="8" t="str">
         <f aca="false">H29</f>
         <v>Dashboard_SI_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>146</v>
+        <v>168</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>169</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
       <c r="F30" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -1958,7 +2099,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H30" s="7" t="str">
+      <c r="H30" s="8" t="str">
         <f aca="false">$I30</f>
         <v>Dashboard_SK_v5.19_PNC_Tra_Int</v>
       </c>
@@ -1966,26 +2107,26 @@
         <f aca="false">"Dashboard_"&amp;$A30&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_SK_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J30" s="7" t="str">
+      <c r="J30" s="8" t="str">
         <f aca="false">H30</f>
         <v>Dashboard_SK_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="F31" s="0" t="b">
         <f aca="false">FALSE()</f>
@@ -1995,7 +2136,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H31" s="7" t="str">
+      <c r="H31" s="8" t="str">
         <f aca="false">$I31</f>
         <v>Dashboard_GB_v5.19_PNC_Tra_Int</v>
       </c>
@@ -2003,20 +2144,20 @@
         <f aca="false">"Dashboard_"&amp;$A31&amp;"_v5.19_PNC_Tra_Int"</f>
         <v>Dashboard_GB_v5.19_PNC_Tra_Int</v>
       </c>
-      <c r="J31" s="5" t="str">
+      <c r="J31" s="6" t="str">
         <f aca="false">H31</f>
         <v>Dashboard_GB_v5.19_PNC_Tra_Int</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>